<commit_message>
Added Raw Data to exampledata.xlsx
Added "First Letter of Cat's Name" and "Cat Age" variables to raw data. Saved updated data to exampledata2.xlsx file.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5B8A21-69CB-CE48-BA5D-B816FD227CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="945" windowWidth="48840" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45600" yWindow="6380" windowWidth="19020" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Height</t>
   </si>
@@ -72,6 +72,42 @@
   </si>
   <si>
     <t>identified gender (male/female/other)</t>
+  </si>
+  <si>
+    <t>First Letter of Cat's Name</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Cat Age (yr)</t>
   </si>
 </sst>
 </file>
@@ -398,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +452,14 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>180</v>
       </c>
@@ -427,8 +469,14 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>175</v>
       </c>
@@ -438,8 +486,14 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -449,8 +503,14 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>178</v>
       </c>
@@ -460,8 +520,14 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>192</v>
       </c>
@@ -471,8 +537,14 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -482,8 +554,14 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>156</v>
       </c>
@@ -493,8 +571,14 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>166</v>
       </c>
@@ -504,8 +588,14 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>155</v>
       </c>
@@ -515,8 +605,14 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>145</v>
       </c>
@@ -526,16 +622,28 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>165</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>133</v>
       </c>
@@ -545,8 +653,14 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>166</v>
       </c>
@@ -556,8 +670,14 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>154</v>
       </c>
@@ -566,6 +686,12 @@
       </c>
       <c r="C15" t="s">
         <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -581,14 +707,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -599,7 +725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -610,7 +736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -621,7 +747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>

</xml_diff>